<commit_message>
FInishing touches on graphs and knitting document
</commit_message>
<xml_diff>
--- a/Tables/Table_2.xlsx
+++ b/Tables/Table_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashaedmondson/Desktop/Environmental_Data_Analytics_2020/FinalProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashaedmondson/Desktop/Environmental_Data_Analytics_2020/FinalProject/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8550737B-647E-F84A-834F-6E6718DFACC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185D30C3-258A-8547-92C0-EBFA2424957D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8980" yWindow="2680" windowWidth="25040" windowHeight="13820" xr2:uid="{CCC76CF3-02D7-3F40-A0E8-EC895223EE4C}"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="25040" windowHeight="13820" xr2:uid="{CCC76CF3-02D7-3F40-A0E8-EC895223EE4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,7 +218,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -226,21 +226,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,19 +575,20 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="66.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -579,7 +596,7 @@
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -587,7 +604,7 @@
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -595,7 +612,7 @@
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -603,7 +620,7 @@
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -611,7 +628,7 @@
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -619,7 +636,7 @@
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -627,7 +644,7 @@
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -635,7 +652,7 @@
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -643,7 +660,7 @@
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -651,7 +668,7 @@
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -659,7 +676,7 @@
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -667,7 +684,7 @@
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -675,7 +692,7 @@
       <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -683,7 +700,7 @@
       <c r="A15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -691,7 +708,7 @@
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -699,7 +716,7 @@
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -707,7 +724,7 @@
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -715,7 +732,7 @@
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -723,7 +740,7 @@
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -731,7 +748,7 @@
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -739,7 +756,7 @@
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -747,7 +764,7 @@
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -755,7 +772,7 @@
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -763,15 +780,15 @@
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>